<commit_message>
Added citation file, fixed gramatical issues, and did a last run through to ensure everything is working.
</commit_message>
<xml_diff>
--- a/dataframes/CX3_radical_dataframe_output.xlsx
+++ b/dataframes/CX3_radical_dataframe_output.xlsx
@@ -758,17 +758,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>Cl</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>Cl</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -817,40 +817,40 @@
         <v>-0.170843</v>
       </c>
       <c r="S2" t="n">
-        <v>0.000187</v>
+        <v>-0.002313</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.000296</v>
+        <v>0.089421</v>
       </c>
       <c r="U2" t="n">
-        <v>6.7e-05</v>
+        <v>0.264311</v>
       </c>
       <c r="V2" t="n">
-        <v>1.05183</v>
+        <v>1.481661</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.242963</v>
+        <v>-0.682382</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.000889</v>
+        <v>-0.079004</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.736138</v>
+        <v>-1.442097</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.789446</v>
+        <v>-0.7627</v>
       </c>
       <c r="AA2" t="n">
-        <v>-0.000193</v>
+        <v>-0.076997</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.31588</v>
+        <v>-0.037251</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.031705</v>
+        <v>1.355661</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.001015</v>
+        <v>-0.10931</v>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
@@ -890,12 +890,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Cl</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>Cl</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -949,40 +949,40 @@
         <v>-0.169773</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.092219</v>
+        <v>-0.000416</v>
       </c>
       <c r="T3" t="n">
-        <v>0.00088</v>
+        <v>0.152737</v>
       </c>
       <c r="U3" t="n">
-        <v>0.109762</v>
+        <v>0.13132</v>
       </c>
       <c r="V3" t="n">
-        <v>1.231268</v>
+        <v>1.463555</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.002992</v>
+        <v>-0.675848</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.033059</v>
+        <v>-0.027898</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.571695</v>
+        <v>-1.458564</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.957187</v>
+        <v>-0.68667</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.031985</v>
+        <v>-0.024772</v>
       </c>
       <c r="AB3" t="n">
-        <v>-0.5673550000000001</v>
+        <v>-0.004576</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.959299</v>
+        <v>1.210782</v>
       </c>
       <c r="AD3" t="n">
-        <v>-0.043718</v>
+        <v>-0.079649</v>
       </c>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
@@ -1022,17 +1022,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Cl</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>F</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>F</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>H</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1081,40 +1081,40 @@
         <v>-0.137996</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.001412</v>
+        <v>-0.103297</v>
       </c>
       <c r="T4" t="n">
-        <v>0.078346</v>
+        <v>0.003684</v>
       </c>
       <c r="U4" t="n">
-        <v>0.242303</v>
+        <v>0.288204</v>
       </c>
       <c r="V4" t="n">
-        <v>1.099869</v>
+        <v>1.576829</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.578467</v>
+        <v>-0.074866</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.074851</v>
+        <v>-0.06643400000000001</v>
       </c>
       <c r="Y4" t="n">
-        <v>-1.080333</v>
+        <v>-0.685325</v>
       </c>
       <c r="Z4" t="n">
-        <v>-0.614307</v>
+        <v>1.114921</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.074653</v>
+        <v>-0.10589</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.018124</v>
+        <v>-0.788206</v>
       </c>
       <c r="AC4" t="n">
-        <v>1.114428</v>
+        <v>-1.043739</v>
       </c>
       <c r="AD4" t="n">
-        <v>-0.09279900000000001</v>
+        <v>-0.114879</v>
       </c>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
@@ -1154,17 +1154,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Cl</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>F</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1213,40 +1213,40 @@
         <v>-0.147709</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.0005240000000000001</v>
+        <v>-0.116008</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.00107</v>
+        <v>0.08973299999999999</v>
       </c>
       <c r="U5" t="n">
-        <v>0.295616</v>
+        <v>0.206337</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.7313460000000001</v>
+        <v>1.531236</v>
       </c>
       <c r="W5" t="n">
-        <v>-1.01609</v>
+        <v>-0.234733</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.102357</v>
+        <v>-0.04213</v>
       </c>
       <c r="Y5" t="n">
-        <v>-0.5142949999999999</v>
+        <v>-0.932765</v>
       </c>
       <c r="Z5" t="n">
-        <v>1.142062</v>
+        <v>-0.917822</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.095357</v>
+        <v>-0.064939</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.246166</v>
+        <v>-0.482463</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.124902</v>
+        <v>1.062822</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.096901</v>
+        <v>-0.099269</v>
       </c>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
@@ -1446,7 +1446,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1505,40 +1505,40 @@
         <v>-0.118083</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.116008</v>
+        <v>-0.0005240000000000001</v>
       </c>
       <c r="T7" t="n">
-        <v>0.08973299999999999</v>
+        <v>-0.00107</v>
       </c>
       <c r="U7" t="n">
-        <v>0.206337</v>
+        <v>0.295616</v>
       </c>
       <c r="V7" t="n">
-        <v>1.531236</v>
+        <v>-0.7313460000000001</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.234733</v>
+        <v>-1.01609</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.04213</v>
+        <v>-0.102357</v>
       </c>
       <c r="Y7" t="n">
-        <v>-0.932765</v>
+        <v>-0.5142949999999999</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.917822</v>
+        <v>1.142062</v>
       </c>
       <c r="AA7" t="n">
-        <v>-0.064939</v>
+        <v>-0.095357</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.482463</v>
+        <v>1.246166</v>
       </c>
       <c r="AC7" t="n">
-        <v>1.062822</v>
+        <v>-0.124902</v>
       </c>
       <c r="AD7" t="n">
-        <v>-0.099269</v>
+        <v>-0.096901</v>
       </c>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
@@ -1578,7 +1578,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -1637,40 +1637,40 @@
         <v>-0.13453</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.103297</v>
+        <v>-0.001412</v>
       </c>
       <c r="T8" t="n">
-        <v>0.003684</v>
+        <v>0.078346</v>
       </c>
       <c r="U8" t="n">
-        <v>0.288204</v>
+        <v>0.242303</v>
       </c>
       <c r="V8" t="n">
-        <v>1.576829</v>
+        <v>1.099869</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.074866</v>
+        <v>-0.578467</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.06643400000000001</v>
+        <v>-0.074851</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.685325</v>
+        <v>-1.080333</v>
       </c>
       <c r="Z8" t="n">
-        <v>1.114921</v>
+        <v>-0.614307</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.10589</v>
+        <v>-0.074653</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.788206</v>
+        <v>-0.018124</v>
       </c>
       <c r="AC8" t="n">
-        <v>-1.043739</v>
+        <v>1.114428</v>
       </c>
       <c r="AD8" t="n">
-        <v>-0.114879</v>
+        <v>-0.09279900000000001</v>
       </c>
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
@@ -1710,12 +1710,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>H</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1769,40 +1769,40 @@
         <v>-0.114953</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.000416</v>
+        <v>-0.092219</v>
       </c>
       <c r="T9" t="n">
-        <v>0.152737</v>
+        <v>0.00088</v>
       </c>
       <c r="U9" t="n">
-        <v>0.13132</v>
+        <v>0.109762</v>
       </c>
       <c r="V9" t="n">
-        <v>1.463555</v>
+        <v>1.231268</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.675848</v>
+        <v>-0.002992</v>
       </c>
       <c r="X9" t="n">
-        <v>-0.027898</v>
+        <v>-0.033059</v>
       </c>
       <c r="Y9" t="n">
-        <v>-1.458564</v>
+        <v>-0.571695</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.68667</v>
+        <v>-0.957187</v>
       </c>
       <c r="AA9" t="n">
-        <v>-0.024772</v>
+        <v>-0.031985</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.004576</v>
+        <v>-0.5673550000000001</v>
       </c>
       <c r="AC9" t="n">
-        <v>1.210782</v>
+        <v>0.959299</v>
       </c>
       <c r="AD9" t="n">
-        <v>-0.079649</v>
+        <v>-0.043718</v>
       </c>
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
@@ -1842,17 +1842,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>H</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cl</t>
+          <t>H</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1901,40 +1901,40 @@
         <v>-0.090022</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.002313</v>
+        <v>0.000187</v>
       </c>
       <c r="T10" t="n">
-        <v>0.089421</v>
+        <v>-0.000296</v>
       </c>
       <c r="U10" t="n">
-        <v>0.264311</v>
+        <v>6.7e-05</v>
       </c>
       <c r="V10" t="n">
-        <v>1.481661</v>
+        <v>1.05183</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.682382</v>
+        <v>-0.242963</v>
       </c>
       <c r="X10" t="n">
-        <v>-0.079004</v>
+        <v>-0.000889</v>
       </c>
       <c r="Y10" t="n">
-        <v>-1.442097</v>
+        <v>-0.736138</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.7627</v>
+        <v>-0.789446</v>
       </c>
       <c r="AA10" t="n">
-        <v>-0.076997</v>
+        <v>-0.000193</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.037251</v>
+        <v>-0.31588</v>
       </c>
       <c r="AC10" t="n">
-        <v>1.355661</v>
+        <v>1.031705</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.10931</v>
+        <v>0.001015</v>
       </c>
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr"/>

</xml_diff>